<commit_message>
added metrics and reformatting
</commit_message>
<xml_diff>
--- a/gym_mujoco_planar_snake/gym_mujoco_planar_snake/HP_Results.xlsx
+++ b/gym_mujoco_planar_snake/gym_mujoco_planar_snake/HP_Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>accuracy</t>
   </si>
@@ -98,6 +98,54 @@
   </si>
   <si>
     <t>Tue Jul 21 23:31:30 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 17:35:12 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 17:37:45 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 17:55:20 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 18:02:30 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 18:58:16 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 18:59:43 2020</t>
+  </si>
+  <si>
+    <t>Wed Jul 22 19:25:35 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 13:56:45 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 14:07:07 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 14:07:32 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 15:08:05 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 15:12:19 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 15:13:24 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 15:14:46 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 15:17:39 2020</t>
+  </si>
+  <si>
+    <t>Thu Jul 23 17:00:02 2020</t>
   </si>
 </sst>
 </file>
@@ -455,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -934,6 +982,374 @@
         <v>27</v>
       </c>
     </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>0.7289727926254272</v>
+      </c>
+      <c r="B23">
+        <v>128</v>
+      </c>
+      <c r="C23">
+        <v>14500</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.5990680456161499</v>
+      </c>
+      <c r="F23">
+        <v>0.001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>0.9688101410865784</v>
+      </c>
+      <c r="B24">
+        <v>128</v>
+      </c>
+      <c r="C24">
+        <v>14500</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>0.5233844518661499</v>
+      </c>
+      <c r="F24">
+        <v>0.0001</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>0.9695556163787842</v>
+      </c>
+      <c r="B25">
+        <v>128</v>
+      </c>
+      <c r="C25">
+        <v>14500</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
+      </c>
+      <c r="E25">
+        <v>0.4996465444564819</v>
+      </c>
+      <c r="F25">
+        <v>0.0001</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>0.9646815657615662</v>
+      </c>
+      <c r="B26">
+        <v>128</v>
+      </c>
+      <c r="C26">
+        <v>14500</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>0.5375465154647827</v>
+      </c>
+      <c r="F26">
+        <v>0.0001</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>0.9731359481811523</v>
+      </c>
+      <c r="B27">
+        <v>128</v>
+      </c>
+      <c r="C27">
+        <v>14500</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>0.4832836389541626</v>
+      </c>
+      <c r="F27">
+        <v>0.0001</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>0.9776589870452881</v>
+      </c>
+      <c r="B28">
+        <v>128</v>
+      </c>
+      <c r="C28">
+        <v>14500</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+      <c r="E28">
+        <v>0.4949248135089874</v>
+      </c>
+      <c r="F28">
+        <v>0.0001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>0.9766995906829834</v>
+      </c>
+      <c r="B29">
+        <v>128</v>
+      </c>
+      <c r="C29">
+        <v>14500</v>
+      </c>
+      <c r="D29">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>0.5067653656005859</v>
+      </c>
+      <c r="F29">
+        <v>0.0001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>0.7157986164093018</v>
+      </c>
+      <c r="B30">
+        <v>128</v>
+      </c>
+      <c r="C30">
+        <v>14500</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.6001615524291992</v>
+      </c>
+      <c r="F30">
+        <v>0.0001</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>0.7362847328186035</v>
+      </c>
+      <c r="B31">
+        <v>128</v>
+      </c>
+      <c r="C31">
+        <v>14500</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0.6436253786087036</v>
+      </c>
+      <c r="F31">
+        <v>0.0001</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>0.8692708611488342</v>
+      </c>
+      <c r="B32">
+        <v>128</v>
+      </c>
+      <c r="C32">
+        <v>14500</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>0.5539892911911011</v>
+      </c>
+      <c r="F32">
+        <v>0.0001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>0.8687499761581421</v>
+      </c>
+      <c r="B33">
+        <v>128</v>
+      </c>
+      <c r="C33">
+        <v>14500</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>0.575569212436676</v>
+      </c>
+      <c r="F33">
+        <v>0.0001</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>0.8763889074325562</v>
+      </c>
+      <c r="B34">
+        <v>128</v>
+      </c>
+      <c r="C34">
+        <v>14500</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>0.5662683844566345</v>
+      </c>
+      <c r="F34">
+        <v>0.0001</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>0.8685764074325562</v>
+      </c>
+      <c r="B35">
+        <v>128</v>
+      </c>
+      <c r="C35">
+        <v>14500</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>0.5539690256118774</v>
+      </c>
+      <c r="F35">
+        <v>0.0001</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>0.8607639074325562</v>
+      </c>
+      <c r="B36">
+        <v>128</v>
+      </c>
+      <c r="C36">
+        <v>14500</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>0.5884552001953125</v>
+      </c>
+      <c r="F36">
+        <v>0.0001</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>0.9710069298744202</v>
+      </c>
+      <c r="B37">
+        <v>128</v>
+      </c>
+      <c r="C37">
+        <v>14500</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
+      </c>
+      <c r="E37">
+        <v>0.5304288864135742</v>
+      </c>
+      <c r="F37">
+        <v>0.0001</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>0.7401041388511658</v>
+      </c>
+      <c r="B38">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>14500</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0.610766589641571</v>
+      </c>
+      <c r="F38">
+        <v>0.0001</v>
+      </c>
+      <c r="G38" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>